<commit_message>
fix style report file
</commit_message>
<xml_diff>
--- a/public/files/reportFile.xlsx
+++ b/public/files/reportFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Server\mini-market-server\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CFAC18-CC54-480B-8BFD-3DBB06306683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AD1E39-B51D-4D91-8F5F-E98C1E6332EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{29FF0485-8FB1-4B0C-9960-B2EAFFB84CE2}"/>
   </bookViews>
@@ -1559,7 +1559,7 @@
     <numFmt numFmtId="167" formatCode="[$-10409]#,##0.000;\(#,##0.000\);\-"/>
     <numFmt numFmtId="168" formatCode="[$-10409]#,##0.00;\(#,##0.00\);\-"/>
   </numFmts>
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1815,12 +1815,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -2070,7 +2064,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2222,6 +2216,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="37" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2257,16 +2260,46 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2295,48 +2328,6 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="37" fontId="40" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="37" fontId="16" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3748,26 +3739,26 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
@@ -3876,89 +3867,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
     </row>
     <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
     </row>
     <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
     </row>
     <row r="5" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
     </row>
     <row r="6" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4114,84 +4105,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
     </row>
     <row r="7" spans="1:14" s="19" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B7" s="20"/>
@@ -4289,17 +4280,17 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
       <c r="J10" s="47"/>
       <c r="K10" s="26"/>
       <c r="L10" s="26"/>
@@ -4364,8 +4355,8 @@
   </sheetPr>
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4394,100 +4385,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
+      <c r="T1" s="73"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
     </row>
     <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
     </row>
     <row r="4" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="68"/>
-      <c r="Q4" s="68"/>
-      <c r="R4" s="68"/>
-      <c r="S4" s="68"/>
-      <c r="T4" s="68"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
     </row>
     <row r="5" spans="1:20" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="70"/>
@@ -4513,30 +4504,30 @@
     </row>
     <row r="6" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D6" s="31"/>
-      <c r="E6" s="88" t="s">
+      <c r="E6" s="74" t="s">
         <v>131</v>
       </c>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="86" t="s">
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="81" t="s">
         <v>133</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="85" t="s">
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="83"/>
+      <c r="N6" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="O6" s="85"/>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="82" t="s">
+      <c r="O6" s="77"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="78" t="s">
         <v>135</v>
       </c>
-      <c r="R6" s="83"/>
-      <c r="S6" s="83"/>
-      <c r="T6" s="84"/>
+      <c r="R6" s="79"/>
+      <c r="S6" s="79"/>
+      <c r="T6" s="80"/>
     </row>
     <row r="7" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
@@ -4629,16 +4620,16 @@
       <c r="J8" s="37"/>
       <c r="K8" s="37"/>
       <c r="L8" s="37"/>
-      <c r="M8" s="92">
+      <c r="M8" s="56">
         <v>11111</v>
       </c>
-      <c r="N8" s="92">
+      <c r="N8" s="56">
         <v>11111</v>
       </c>
-      <c r="O8" s="92">
+      <c r="O8" s="56">
         <v>11111</v>
       </c>
-      <c r="P8" s="92">
+      <c r="P8" s="56">
         <v>11111</v>
       </c>
       <c r="Q8" s="37"/>
@@ -4648,7 +4639,7 @@
       <c r="S8" s="37">
         <v>15</v>
       </c>
-      <c r="T8" s="92">
+      <c r="T8" s="56">
         <v>11111</v>
       </c>
     </row>
@@ -4656,41 +4647,41 @@
       <c r="A9" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="91"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
-      <c r="I9" s="93">
+      <c r="I9" s="57">
         <v>11111</v>
       </c>
       <c r="J9" s="33"/>
       <c r="K9" s="33"/>
       <c r="L9" s="33"/>
-      <c r="M9" s="94">
+      <c r="M9" s="57">
         <v>11111</v>
       </c>
-      <c r="N9" s="94">
+      <c r="N9" s="57">
         <v>11111</v>
       </c>
-      <c r="O9" s="94">
+      <c r="O9" s="57">
         <v>11111</v>
       </c>
-      <c r="P9" s="94">
+      <c r="P9" s="57">
         <v>11111</v>
       </c>
-      <c r="Q9" s="94">
+      <c r="Q9" s="57">
         <v>11111</v>
       </c>
-      <c r="R9" s="94">
+      <c r="R9" s="57">
         <v>11111</v>
       </c>
-      <c r="S9" s="94">
+      <c r="S9" s="57">
         <v>11111</v>
       </c>
-      <c r="T9" s="94">
+      <c r="T9" s="57">
         <v>11111</v>
       </c>
     </row>
@@ -4704,15 +4695,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="J6:M6"/>
     <mergeCell ref="A5:T5"/>
     <mergeCell ref="A3:T3"/>
     <mergeCell ref="A4:T4"/>
     <mergeCell ref="A2:T2"/>
     <mergeCell ref="A1:T1"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="J6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4743,54 +4734,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
     </row>
     <row r="4" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
     </row>
     <row r="6" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
     </row>
     <row r="7" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.25">
@@ -4838,14 +4829,14 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="72"/>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
-      <c r="E10" s="72"/>
-      <c r="F10" s="73"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="86"/>
       <c r="G10" s="17">
         <v>0</v>
       </c>
@@ -4899,141 +4890,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="90" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
     </row>
     <row r="2" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
     </row>
     <row r="3" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="M3" s="78"/>
-      <c r="N3" s="78"/>
-      <c r="O3" s="78"/>
-      <c r="P3" s="78"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
     </row>
     <row r="4" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
     </row>
     <row r="5" spans="1:17" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
     </row>
     <row r="6" spans="1:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="78"/>
-      <c r="K6" s="78"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="78"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
     </row>
     <row r="7" spans="1:17" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I7" s="76" t="s">
+      <c r="I7" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76" t="s">
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="89" t="s">
         <v>75</v>
       </c>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76" t="s">
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
+      <c r="P7" s="89"/>
+      <c r="Q7" s="89"/>
     </row>
     <row r="8" spans="1:17" ht="33" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
@@ -5134,15 +5125,15 @@
       <c r="Q9" s="44"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="87" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
       <c r="H10" s="45"/>
       <c r="I10" s="46"/>
       <c r="J10" s="46"/>

</xml_diff>